<commit_message>
First player activation and colour choice
Codded but not yet debuged
</commit_message>
<xml_diff>
--- a/PossibleStartingScreen.xlsx
+++ b/PossibleStartingScreen.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MesChoses\Autres\Github\multiplayerSnake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327FAD9F-8C4D-48AC-9A80-A5B875FF264E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0176855B-C09C-4FA4-B63A-7D8BAAFD877E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CA1E80F-696C-4149-87A2-9728D32DECC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -565,16 +565,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412CFC93-C3A4-4E96-AFC8-C2E965482321}">
   <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="32" width="3.7109375" customWidth="1"/>
+    <col min="1" max="32" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -796,10 +796,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
@@ -823,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="R3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="1">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="1">
         <v>0</v>
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -918,10 +918,10 @@
         <v>1</v>
       </c>
       <c r="Q4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="AA4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="1">
         <v>0</v>
@@ -966,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
@@ -1028,25 +1028,25 @@
         <v>0</v>
       </c>
       <c r="U5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" s="1">
         <v>0</v>
       </c>
       <c r="W5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="1">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -1126,25 +1126,25 @@
         <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1">
         <v>1</v>
       </c>
       <c r="X6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="1">
         <v>0</v>
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="W7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" s="1">
         <v>0</v>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1307,28 +1307,28 @@
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
@@ -1358,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" s="1">
         <v>0</v>
@@ -2605,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="1">
         <v>0</v>
@@ -2623,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="AD21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21" s="1">
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="T22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" s="1">
         <v>0</v>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="X22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22" s="1">
         <v>0</v>
@@ -2721,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="AD22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE22" s="1">
         <v>0</v>
@@ -2730,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="1">
         <v>0</v>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="X23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="1">
         <v>0</v>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="AD23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23" s="1">
         <v>0</v>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -2890,16 +2890,16 @@
         <v>1</v>
       </c>
       <c r="U24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="1">
         <v>0</v>
@@ -2926,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -3711,7 +3711,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AF11 A18:AF32 A12:F17 AA12:AF17 G13:Z17">
+  <conditionalFormatting sqref="A12:F17 AA12:AF17 G13:Z17 A18:AF32 A1:AF11">
     <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
Bugfix and improving player colour selection
</commit_message>
<xml_diff>
--- a/PossibleStartingScreen.xlsx
+++ b/PossibleStartingScreen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MesChoses\Autres\Github\multiplayerSnake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0176855B-C09C-4FA4-B63A-7D8BAAFD877E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BA7D79-F6E1-4396-8FDA-4452D9C580F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CA1E80F-696C-4149-87A2-9728D32DECC1}"/>
   </bookViews>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412CFC93-C3A4-4E96-AFC8-C2E965482321}">
   <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="AD23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE23" s="1">
         <v>0</v>
@@ -3711,7 +3711,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A12:F17 AA12:AF17 G13:Z17 A18:AF32 A1:AF11">
+  <conditionalFormatting sqref="A12:F17 AA12:AF17 G13:Z17 A1:AF11 A18:AF32">
     <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>10</formula>
     </cfRule>

</xml_diff>